<commit_message>
Entidades obra y referente modeladas en tablas diferentes
</commit_message>
<xml_diff>
--- a/data/bga-obra.xlsx
+++ b/data/bga-obra.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gemartin/diseno-proyectos/sesiones/agile-dh/bga-archivos-iniciales/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gemartin/diseno-proyectos/sesiones/agile-dh/bga-obra/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EA63386-FCE5-304E-B937-1A3A2E47B065}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{ED3DECAD-3237-C84E-9BBF-1CB9CD44D9AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55120" yWindow="-9380" windowWidth="34540" windowHeight="26040" xr2:uid="{8E12BB4E-903A-BD4F-8671-6F5A3A14E5C1}"/>
+    <workbookView xWindow="-47020" yWindow="-8760" windowWidth="34540" windowHeight="26040" activeTab="1" xr2:uid="{8E12BB4E-903A-BD4F-8671-6F5A3A14E5C1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="bga-obra" sheetId="1" r:id="rId1"/>
+    <sheet name="obra" sheetId="4" r:id="rId2"/>
+    <sheet name="referente" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -465,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A02C49DC-5823-D94A-9982-F309D43F69BF}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,4 +622,199 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07830450-B7E1-7E43-9844-CA2C8C1B3037}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="25.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>1965</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>1997</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>1983</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{702222AF-09A9-8E45-95E4-8797A37D87E5}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="35.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implementado Dublin Core en tablas
</commit_message>
<xml_diff>
--- a/data/bga-obra.xlsx
+++ b/data/bga-obra.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gemartin/diseno-proyectos/sesiones/agile-dh/bga-obra/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{ED3DECAD-3237-C84E-9BBF-1CB9CD44D9AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E033DF5E-B332-A047-96E2-566D2D24B8D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-47020" yWindow="-8760" windowWidth="34540" windowHeight="26040" activeTab="1" xr2:uid="{8E12BB4E-903A-BD4F-8671-6F5A3A14E5C1}"/>
+    <workbookView xWindow="-50260" yWindow="-9420" windowWidth="34540" windowHeight="26040" xr2:uid="{8E12BB4E-903A-BD4F-8671-6F5A3A14E5C1}"/>
   </bookViews>
   <sheets>
-    <sheet name="bga-obra" sheetId="1" r:id="rId1"/>
-    <sheet name="obra" sheetId="4" r:id="rId2"/>
-    <sheet name="referente" sheetId="5" r:id="rId3"/>
+    <sheet name="obra" sheetId="4" r:id="rId1"/>
+    <sheet name="referente" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,26 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Título</t>
-  </si>
-  <si>
-    <t>Fecha</t>
-  </si>
-  <si>
-    <t>Dimensiones</t>
-  </si>
-  <si>
-    <t>Técnica</t>
-  </si>
-  <si>
-    <t>Periódico</t>
-  </si>
-  <si>
     <t>Archivo</t>
   </si>
   <si>
@@ -114,6 +98,21 @@
   </si>
   <si>
     <t>exmilitar-mata-esposa.jpg</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Publisher</t>
   </si>
 </sst>
 </file>
@@ -464,172 +463,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A02C49DC-5823-D94A-9982-F309D43F69BF}">
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="25.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>1965</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4">
-        <v>1997</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7">
-        <v>1983</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07830450-B7E1-7E43-9844-CA2C8C1B3037}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,19 +484,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -666,19 +504,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>1965</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -686,19 +524,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>1997</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -706,19 +544,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>1983</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -726,12 +564,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{702222AF-09A9-8E45-95E4-8797A37D87E5}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -746,16 +584,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -763,16 +601,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -780,16 +618,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -797,10 +635,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -808,10 +646,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>